<commit_message>
The project has been verified and uploaded successfully
</commit_message>
<xml_diff>
--- a/Reports_files/Automation_Testing_testcases.xlsx
+++ b/Reports_files/Automation_Testing_testcases.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="333">
   <si>
     <t>Test Scenario Description</t>
   </si>
@@ -404,9 +404,6 @@
     <t>Unsuccessful login with invalid mobile number</t>
   </si>
   <si>
-    <t xml:space="preserve"> When the user enters invalid mobileno as "&lt;Mobile_No&gt;"</t>
-  </si>
-  <si>
     <t>And the user clicks the continue button</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
   </si>
   <si>
     <t>Sub story 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Given the user is on the homepage</t>
   </si>
   <si>
     <t>And the user enters origin as "&lt;from&gt;"</t>
@@ -1071,34 +1065,49 @@
     <t>User should be able to enter destination location.</t>
   </si>
   <si>
-    <t xml:space="preserve">  user sets travellers as "&lt;adults&gt;" adults, "&lt;children&gt;" children, "&lt;infants&gt;" infants and class as "&lt;travel_class&gt;"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> user clicks Search</t>
-  </si>
-  <si>
     <t xml:space="preserve"> search results should be displayed</t>
   </si>
   <si>
-    <t xml:space="preserve"> the user is on the login page</t>
-  </si>
-  <si>
     <t>the user clicks the offer icon</t>
   </si>
   <si>
-    <t xml:space="preserve">  the user selects the dropdown More option</t>
-  </si>
-  <si>
     <t>selects tripType trip type</t>
   </si>
   <si>
-    <t xml:space="preserve"> selects from as "&lt;from&gt;" </t>
-  </si>
-  <si>
-    <t>user gives the location where as "&lt;where&gt;"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> user selects the things to do option </t>
+    <t xml:space="preserve"> User sets travellers as adults, children,  infants and class </t>
+  </si>
+  <si>
+    <t>User clicks Search icon</t>
+  </si>
+  <si>
+    <t>User is on the selection page</t>
+  </si>
+  <si>
+    <t>selects the first available flight</t>
+  </si>
+  <si>
+    <t>Select from location</t>
+  </si>
+  <si>
+    <t>Select the to location</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User selects the things to do option </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the user clicks departure filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the user clicks the arrival filter</t>
+  </si>
+  <si>
+    <t>user selects the dropdown More option</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> user is on the login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> user is on the homepage</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1727,7 @@
   <dimension ref="A1:D9671"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1773,13 +1782,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>112</v>
+        <v>331</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
@@ -1787,13 +1796,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -1801,13 +1810,13 @@
     </row>
     <row r="6" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>10</v>
@@ -1815,13 +1824,13 @@
     </row>
     <row r="7" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>10</v>
@@ -1843,13 +1852,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>112</v>
+        <v>331</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>10</v>
@@ -1857,13 +1866,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>10</v>
@@ -1871,13 +1880,13 @@
     </row>
     <row r="11" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>10</v>
@@ -1885,13 +1894,13 @@
     </row>
     <row r="12" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>10</v>
@@ -1905,7 +1914,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>21</v>
@@ -1913,13 +1922,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>123</v>
+        <v>332</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>21</v>
@@ -1927,13 +1936,13 @@
     </row>
     <row r="15" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>21</v>
@@ -1941,13 +1950,13 @@
     </row>
     <row r="16" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>10</v>
@@ -1955,13 +1964,13 @@
     </row>
     <row r="17" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>10</v>
@@ -1969,13 +1978,13 @@
     </row>
     <row r="18" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>10</v>
@@ -1983,13 +1992,13 @@
     </row>
     <row r="19" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D19" s="13" t="s">
         <v>10</v>
@@ -1997,13 +2006,13 @@
     </row>
     <row r="20" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>10</v>
@@ -2017,7 +2026,7 @@
         <v>36</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>10</v>
@@ -2025,7 +2034,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>7</v>
@@ -2039,13 +2048,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>117</v>
+        <v>328</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>10</v>
@@ -2053,13 +2062,13 @@
     </row>
     <row r="24" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>118</v>
+        <v>329</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>10</v>
@@ -2067,13 +2076,13 @@
     </row>
     <row r="25" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>119</v>
+        <v>324</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>10</v>
@@ -2087,7 +2096,7 @@
         <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>10</v>
@@ -2095,13 +2104,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>21</v>
@@ -2109,13 +2118,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>21</v>
@@ -2123,13 +2132,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>109</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="D29" s="13" t="s">
         <v>21</v>
@@ -2137,13 +2146,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>21</v>
@@ -2151,13 +2160,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>21</v>
@@ -2165,13 +2174,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>21</v>
@@ -12019,19 +12028,19 @@
         <v>112</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>40</v>
@@ -12049,36 +12058,36 @@
         <v>113</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F3" s="7">
         <v>8438542755</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H3" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>269</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>270</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>40</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>41</v>
@@ -12087,19 +12096,19 @@
         <v>114</v>
       </c>
       <c r="D4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>139</v>
-      </c>
       <c r="G4" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I4" s="20" t="s">
         <v>40</v>
@@ -12107,7 +12116,7 @@
     </row>
     <row r="5" spans="1:15" s="7" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>41</v>
@@ -12116,19 +12125,19 @@
         <v>115</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I5" s="20" t="s">
         <v>40</v>
@@ -12145,19 +12154,19 @@
         <v>112</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>32</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I6" s="20" t="s">
         <v>40</v>
@@ -12171,22 +12180,22 @@
         <v>42</v>
       </c>
       <c r="C7" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>163</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>40</v>
@@ -12200,22 +12209,22 @@
         <v>42</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="I8" s="20" t="s">
         <v>40</v>
@@ -12229,22 +12238,22 @@
         <v>42</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I9" s="20" t="s">
         <v>40</v>
@@ -12258,22 +12267,22 @@
         <v>43</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I10" s="20" t="s">
         <v>40</v>
@@ -12287,22 +12296,22 @@
         <v>43</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I11" s="20" t="s">
         <v>40</v>
@@ -12316,34 +12325,34 @@
         <v>43</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K12" s="20" t="s">
         <v>40</v>
       </c>
       <c r="N12" s="39" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -12354,40 +12363,40 @@
         <v>43</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I13" s="20" t="s">
         <v>40</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K13" s="38" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M13" s="20" t="s">
         <v>40</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="7" customFormat="1" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -12398,22 +12407,22 @@
         <v>43</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I14" s="20" t="s">
         <v>40</v>
@@ -12421,28 +12430,28 @@
     </row>
     <row r="15" spans="1:15" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I15" s="20" t="s">
         <v>40</v>
@@ -12450,28 +12459,28 @@
     </row>
     <row r="16" spans="1:15" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I16" s="20" t="s">
         <v>40</v>
@@ -12485,22 +12494,22 @@
         <v>44</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I17" s="20" t="s">
         <v>40</v>
@@ -12508,28 +12517,28 @@
     </row>
     <row r="18" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I18" s="20" t="s">
         <v>40</v>
@@ -12537,28 +12546,28 @@
     </row>
     <row r="19" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I19" s="20" t="s">
         <v>40</v>
@@ -12566,28 +12575,28 @@
     </row>
     <row r="20" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I20" s="20" t="s">
         <v>40</v>
@@ -12601,22 +12610,22 @@
         <v>45</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I21" s="20" t="s">
         <v>40</v>
@@ -12624,28 +12633,28 @@
     </row>
     <row r="22" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I22" s="20" t="s">
         <v>40</v>
@@ -12653,66 +12662,66 @@
     </row>
     <row r="23" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I23" s="38" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="K23" s="20" t="s">
         <v>40</v>
       </c>
       <c r="N23" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I24" s="20" t="s">
         <v>40</v>
@@ -12720,28 +12729,28 @@
     </row>
     <row r="25" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I25" s="20" t="s">
         <v>40</v>
@@ -12749,28 +12758,28 @@
     </row>
     <row r="26" spans="1:14" s="7" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I26" s="20" t="s">
         <v>40</v>
@@ -13385,7 +13394,7 @@
         <v>72</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -13405,7 +13414,7 @@
         <v>72</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -13425,7 +13434,7 @@
         <v>72</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -13507,7 +13516,7 @@
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>77</v>
@@ -13520,7 +13529,7 @@
       <c r="A5" s="40"/>
       <c r="B5" s="40"/>
       <c r="C5" s="34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" s="25" t="s">
         <v>79</v>
@@ -13658,7 +13667,7 @@
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15" s="34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>77</v>
@@ -13671,7 +13680,7 @@
       <c r="A16" s="40"/>
       <c r="B16" s="40"/>
       <c r="C16" s="34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D16" s="27" t="s">
         <v>77</v>
@@ -13701,7 +13710,7 @@
       <c r="A18" s="40"/>
       <c r="B18" s="40"/>
       <c r="C18" s="34" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D18" s="27" t="s">
         <v>77</v>
@@ -13714,7 +13723,7 @@
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
       <c r="C19" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D19" s="27" t="s">
         <v>77</v>
@@ -13727,7 +13736,7 @@
       <c r="A20" s="40"/>
       <c r="B20" s="40"/>
       <c r="C20" s="34" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>77</v>
@@ -13757,7 +13766,7 @@
       <c r="A22" s="40"/>
       <c r="B22" s="40"/>
       <c r="C22" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D22" s="27" t="s">
         <v>77</v>
@@ -13770,7 +13779,7 @@
       <c r="A23" s="40"/>
       <c r="B23" s="40"/>
       <c r="C23" s="34" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D23" s="27" t="s">
         <v>77</v>
@@ -13783,7 +13792,7 @@
       <c r="A24" s="40"/>
       <c r="B24" s="40"/>
       <c r="C24" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" s="27" t="s">
         <v>77</v>
@@ -13796,7 +13805,7 @@
       <c r="A25" s="40"/>
       <c r="B25" s="40"/>
       <c r="C25" s="34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>77</v>
@@ -13809,7 +13818,7 @@
       <c r="A26" s="40"/>
       <c r="B26" s="40"/>
       <c r="C26" s="34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D26" s="27" t="s">
         <v>77</v>
@@ -13820,16 +13829,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="B10:B16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13984,7 +13993,7 @@
         <v>90</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C3" s="32">
         <v>4</v>
@@ -14011,7 +14020,7 @@
     <row r="4" spans="1:89" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="43"/>
       <c r="B4" s="24" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C4" s="32">
         <v>4</v>
@@ -14038,7 +14047,7 @@
     <row r="5" spans="1:89" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="43"/>
       <c r="B5" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C5" s="32">
         <v>7</v>
@@ -14065,7 +14074,7 @@
     <row r="6" spans="1:89" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="43"/>
       <c r="B6" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C6" s="32">
         <v>4</v>
@@ -14092,7 +14101,7 @@
     <row r="7" spans="1:89" s="24" customFormat="1" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="43"/>
       <c r="B7" s="24" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C7" s="32">
         <v>6</v>

</xml_diff>